<commit_message>
Add 'mstate_nma_hr', which is output of hazard ratios by month for 1L treatments relative to gefitinib
</commit_message>
<xml_diff>
--- a/data-raw/mstate-nma/params-lookup-1L.xlsx
+++ b/data-raw/mstate-nma/params-lookup-1L.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="25660" windowHeight="14640" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="weibull" sheetId="2" r:id="rId1"/>
@@ -573,7 +573,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -688,9 +688,6 @@
       </c>
       <c r="D6">
         <v>1</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -728,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -840,9 +837,6 @@
       </c>
       <c r="D6">
         <v>2</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -881,7 +875,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1023,9 +1017,6 @@
       </c>
       <c r="D8">
         <v>1</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
       </c>
       <c r="F8">
         <v>5</v>
@@ -1077,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1217,9 +1208,6 @@
       </c>
       <c r="D8">
         <v>1</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
       </c>
       <c r="F8">
         <v>5</v>

</xml_diff>

<commit_message>
Add coefficient tables from multistate NMA and MA
</commit_message>
<xml_diff>
--- a/data-raw/mstate-nma/params-lookup-1L.xlsx
+++ b/data-raw/mstate-nma/params-lookup-1L.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="25660" windowHeight="14640" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="280" yWindow="220" windowWidth="25040" windowHeight="14060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="weibull" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="26">
   <si>
     <t>transition</t>
   </si>
@@ -70,6 +70,36 @@
   </si>
   <si>
     <t>transition_id</t>
+  </si>
+  <si>
+    <t>d_name</t>
+  </si>
+  <si>
+    <t>mu_name</t>
+  </si>
+  <si>
+    <t>d_1</t>
+  </si>
+  <si>
+    <t>d_2</t>
+  </si>
+  <si>
+    <t>mu_1</t>
+  </si>
+  <si>
+    <t>mu_2</t>
+  </si>
+  <si>
+    <t>mu_3</t>
+  </si>
+  <si>
+    <t>mu_5</t>
+  </si>
+  <si>
+    <t>mu_6</t>
+  </si>
+  <si>
+    <t>mu_4</t>
   </si>
 </sst>
 </file>
@@ -118,7 +148,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -177,12 +207,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="60">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -212,6 +243,7 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -570,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -585,7 +617,7 @@
     <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,8 +636,14 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -624,8 +662,14 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -644,8 +688,14 @@
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -661,8 +711,11 @@
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -676,7 +729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -692,8 +745,11 @@
       <c r="F6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -708,6 +764,9 @@
       </c>
       <c r="F7">
         <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -723,10 +782,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -734,7 +793,7 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -753,8 +812,14 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -773,8 +838,14 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -793,8 +864,14 @@
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -810,8 +887,11 @@
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -825,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -841,8 +921,11 @@
       <c r="F6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -857,6 +940,9 @@
       </c>
       <c r="F7">
         <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -872,10 +958,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G1" sqref="G1:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -883,7 +969,7 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -902,8 +988,14 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -922,8 +1014,14 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -942,8 +1040,14 @@
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -959,8 +1063,11 @@
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -976,8 +1083,11 @@
       <c r="F5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -991,7 +1101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1005,7 +1115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1021,8 +1131,11 @@
       <c r="F8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1038,8 +1151,11 @@
       <c r="F9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1066,15 +1182,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1093,8 +1209,14 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1113,8 +1235,14 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1133,8 +1261,14 @@
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1150,8 +1284,11 @@
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1167,8 +1304,11 @@
       <c r="F5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1182,7 +1322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1196,7 +1336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1212,8 +1352,11 @@
       <c r="F8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1229,8 +1372,11 @@
       <c r="F9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Update NMA and MA coefficient tables to use M instead of mu for consistency with the PDF documentation
</commit_message>
<xml_diff>
--- a/data-raw/mstate-nma/params-lookup-1L.xlsx
+++ b/data-raw/mstate-nma/params-lookup-1L.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="220" windowWidth="25040" windowHeight="14060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="280" yWindow="220" windowWidth="25040" windowHeight="14060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="weibull" sheetId="2" r:id="rId1"/>
@@ -84,22 +84,22 @@
     <t>d_2</t>
   </si>
   <si>
-    <t>mu_1</t>
-  </si>
-  <si>
-    <t>mu_2</t>
-  </si>
-  <si>
-    <t>mu_3</t>
-  </si>
-  <si>
-    <t>mu_5</t>
-  </si>
-  <si>
-    <t>mu_6</t>
-  </si>
-  <si>
-    <t>mu_4</t>
+    <t>M_1</t>
+  </si>
+  <si>
+    <t>M_2</t>
+  </si>
+  <si>
+    <t>M_4</t>
+  </si>
+  <si>
+    <t>M_5</t>
+  </si>
+  <si>
+    <t>M_6</t>
+  </si>
+  <si>
+    <t>M_3</t>
   </si>
 </sst>
 </file>
@@ -148,7 +148,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="60">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -208,12 +208,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="60">
+  <cellStyles count="62">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -244,6 +246,7 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -273,6 +276,7 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,7 +609,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -712,7 +716,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -784,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -888,7 +892,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -961,7 +965,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1064,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1084,7 +1088,7 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1184,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1285,7 +1289,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1305,7 +1309,7 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8">

</xml_diff>